<commit_message>
Discussion results educational categories
</commit_message>
<xml_diff>
--- a/conversions.xlsx
+++ b/conversions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eui1-my.sharepoint.com/personal/alessandro_ferrara_eui_eu/Documents/Documents/GitHub/CILS4EU_mig/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\husowi28c.user.hu-berlin.de\SowiHome\hornunma\Eigene Dateien\GitHub\CILS4EU_mig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="11_AD4DB114E441178AC67DF4035ED6D1A8683EDF24" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C483D1A8-72D3-4D6B-8B1E-1AFA4C07A3FD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605A0817-DD3F-4748-86DF-D5D0665F31B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-5830" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="84">
   <si>
     <t xml:space="preserve">    38 "other activity" , modify </t>
   </si>
@@ -175,6 +175,108 @@
   </si>
   <si>
     <t>Employed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upper secondary </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combined all </t>
+  </si>
+  <si>
+    <t>do robustness checks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other </t>
+  </si>
+  <si>
+    <t xml:space="preserve">optimistic </t>
+  </si>
+  <si>
+    <t>combined</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other </t>
+  </si>
+  <si>
+    <t xml:space="preserve">recode </t>
+  </si>
+  <si>
+    <t>Evening lower secondary school</t>
+  </si>
+  <si>
+    <t>Evening intermediate secondary school</t>
+  </si>
+  <si>
+    <t>Evening upper secondary school</t>
+  </si>
+  <si>
+    <t>Other evening school (andere Abendschule) 4</t>
+  </si>
+  <si>
+    <t>Folk high school (Volkshochschule) 5</t>
+  </si>
+  <si>
+    <t>Vocational extension school</t>
+  </si>
+  <si>
+    <t>School for continuing vocational training</t>
+  </si>
+  <si>
+    <t>Vocational college (Berufskolleg) 8</t>
+  </si>
+  <si>
+    <t>Higher secondary vocational school</t>
+  </si>
+  <si>
+    <t>Distance learning school (Fernschule) 10</t>
+  </si>
+  <si>
+    <t>(Fachgymnasium/berufliches Gymnasium) 12</t>
+  </si>
+  <si>
+    <t>Adult education college (Kolleg) 13</t>
+  </si>
+  <si>
+    <t>Remote adult education college (Telekolleg) 14</t>
+  </si>
+  <si>
+    <t>Other type of school 15</t>
+  </si>
+  <si>
+    <t>lower secondary</t>
+  </si>
+  <si>
+    <t>intermediate secondary</t>
+  </si>
+  <si>
+    <t>Tertiary</t>
+  </si>
+  <si>
+    <t>Employment</t>
+  </si>
+  <si>
+    <t>Out of employment</t>
+  </si>
+  <si>
+    <t>upper secondary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">upper secondary </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recoding second chance education </t>
+  </si>
+  <si>
+    <t xml:space="preserve">robustness variable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">always prioritize education </t>
+  </si>
+  <si>
+    <t xml:space="preserve">apprenticeship </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prioritize the highest (education) </t>
   </si>
 </sst>
 </file>
@@ -198,7 +300,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,6 +310,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -224,12 +332,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,294 +620,581 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="114.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.73046875" customWidth="1"/>
+    <col min="1" max="1" width="125.08984375" customWidth="1"/>
+    <col min="2" max="2" width="49.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C25" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C26" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="C32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="C33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="C34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="C35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="C36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="C37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="C38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>0</v>
       </c>
+      <c r="C39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>66</v>
+      </c>
+      <c r="C53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>69</v>
+      </c>
+      <c r="C55" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>71</v>
+      </c>
+      <c r="C57" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B61" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B62" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>